<commit_message>
Universal Code edit 3
</commit_message>
<xml_diff>
--- a/Facility_Staffing_Combined.xlsx
+++ b/Facility_Staffing_Combined.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keros\.venv\Capstone-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C097E90A-0DD6-44DC-83E9-5B578F59AD53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A70477E-54D2-434F-BC94-F8D8BB237353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28545" yWindow="15480" windowWidth="16410" windowHeight="11295" xr2:uid="{0B339019-6CC6-4650-AC0A-9ED3E400C083}"/>
+    <workbookView xWindow="-16320" yWindow="-120" windowWidth="16440" windowHeight="28320" xr2:uid="{0B339019-6CC6-4650-AC0A-9ED3E400C083}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -582,7 +582,7 @@
   <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="L58" sqref="L58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2674,5 +2674,227 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
+      <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{290A9256-DC15-46CF-A6E5-BB06CCE0323F}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Sheet1!B2:J2</xm:f>
+              <xm:sqref>M2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B3:J3</xm:f>
+              <xm:sqref>M3</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B4:J4</xm:f>
+              <xm:sqref>M4</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B5:J5</xm:f>
+              <xm:sqref>M5</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B6:J6</xm:f>
+              <xm:sqref>M6</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B7:J7</xm:f>
+              <xm:sqref>M7</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B8:J8</xm:f>
+              <xm:sqref>M8</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B9:J9</xm:f>
+              <xm:sqref>M9</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B10:J10</xm:f>
+              <xm:sqref>M10</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B11:J11</xm:f>
+              <xm:sqref>M11</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B12:J12</xm:f>
+              <xm:sqref>M12</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B13:J13</xm:f>
+              <xm:sqref>M13</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B14:J14</xm:f>
+              <xm:sqref>M14</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B15:J15</xm:f>
+              <xm:sqref>M15</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B16:J16</xm:f>
+              <xm:sqref>M16</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B17:J17</xm:f>
+              <xm:sqref>M17</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B18:J18</xm:f>
+              <xm:sqref>M18</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B19:J19</xm:f>
+              <xm:sqref>M19</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B20:J20</xm:f>
+              <xm:sqref>M20</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B21:J21</xm:f>
+              <xm:sqref>M21</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B22:J22</xm:f>
+              <xm:sqref>M22</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B23:J23</xm:f>
+              <xm:sqref>M23</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B24:J24</xm:f>
+              <xm:sqref>M24</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B25:J25</xm:f>
+              <xm:sqref>M25</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B26:J26</xm:f>
+              <xm:sqref>M26</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B27:J27</xm:f>
+              <xm:sqref>M27</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B28:J28</xm:f>
+              <xm:sqref>M28</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B29:J29</xm:f>
+              <xm:sqref>M29</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B30:J30</xm:f>
+              <xm:sqref>M30</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B31:J31</xm:f>
+              <xm:sqref>M31</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B32:J32</xm:f>
+              <xm:sqref>M32</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B33:J33</xm:f>
+              <xm:sqref>M33</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B34:J34</xm:f>
+              <xm:sqref>M34</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B35:J35</xm:f>
+              <xm:sqref>M35</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B36:J36</xm:f>
+              <xm:sqref>M36</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B37:J37</xm:f>
+              <xm:sqref>M37</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B38:J38</xm:f>
+              <xm:sqref>M38</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B39:J39</xm:f>
+              <xm:sqref>M39</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B40:J40</xm:f>
+              <xm:sqref>M40</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B41:J41</xm:f>
+              <xm:sqref>M41</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B42:J42</xm:f>
+              <xm:sqref>M42</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B43:J43</xm:f>
+              <xm:sqref>M43</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B44:J44</xm:f>
+              <xm:sqref>M44</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B45:J45</xm:f>
+              <xm:sqref>M45</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B46:J46</xm:f>
+              <xm:sqref>M46</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B47:J47</xm:f>
+              <xm:sqref>M47</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B48:J48</xm:f>
+              <xm:sqref>M48</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B49:J49</xm:f>
+              <xm:sqref>M49</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B50:J50</xm:f>
+              <xm:sqref>M50</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B51:J51</xm:f>
+              <xm:sqref>M51</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B52:J52</xm:f>
+              <xm:sqref>M52</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+      </x14:sparklineGroups>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>